<commit_message>
finalise mood's median test
</commit_message>
<xml_diff>
--- a/statistical-analysis/Performance t-test.xlsx
+++ b/statistical-analysis/Performance t-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgray/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylorgray/lighthouse-audit/statistical-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8212BCA5-F580-E146-98A5-9DDA83518C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0FDE0A-11E4-4E44-B7CD-87F49DFAC757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21200" tabRatio="845" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="40960" windowHeight="23040" tabRatio="845" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Non-Parametric Tests" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="E4" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -406,8 +406,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="260">
   <si>
     <t>Samples</t>
   </si>
@@ -1228,9 +1250,6 @@
     <t>Sum</t>
   </si>
   <si>
-    <t>Chi-Sq</t>
-  </si>
-  <si>
     <t>Mood's Median Test</t>
   </si>
   <si>
@@ -1245,6 +1264,33 @@
   <si>
     <t>React</t>
   </si>
+  <si>
+    <t>Observed Frequencies</t>
+  </si>
+  <si>
+    <t>Expected Frequencies</t>
+  </si>
+  <si>
+    <t>Chi-Sq O</t>
+  </si>
+  <si>
+    <t>Chi-Sq Crit</t>
+  </si>
+  <si>
+    <t>Freq r</t>
+  </si>
+  <si>
+    <t>Bins r</t>
+  </si>
+  <si>
+    <t>Bins a</t>
+  </si>
+  <si>
+    <t>Freq a</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
 </sst>
 </file>
 
@@ -1254,7 +1300,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="62" x14ac:knownFonts="1">
+  <fonts count="66" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1293,6 +1339,7 @@
     <font>
       <sz val="10"/>
       <name val="Times"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -1340,6 +1387,7 @@
     <font>
       <sz val="10"/>
       <name val="Geneva"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1499,6 +1547,7 @@
       <sz val="8.5"/>
       <color indexed="12"/>
       <name val="Geneva"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1506,6 +1555,7 @@
       <sz val="12"/>
       <color theme="0"/>
       <name val="Geneva"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1561,6 +1611,7 @@
       <b/>
       <sz val="10"/>
       <name val="Geneva"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1581,6 +1632,7 @@
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Geneva"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1657,6 +1709,31 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF00FFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -2443,7 +2520,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="336">
+  <cellXfs count="354">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3004,7 +3081,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="50"/>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="50" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="22" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
@@ -3012,31 +3088,12 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="50" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="58" fillId="29" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="58" fillId="31" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="58" fillId="31" borderId="10" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="58" fillId="28" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="57" fillId="26" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="26" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="56" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="59" fillId="26" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="58" fillId="31" borderId="10" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="60" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="58" fillId="30" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="57" fillId="26" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="58" fillId="31" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="58" fillId="31" borderId="30" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="34" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3074,6 +3131,80 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="26" borderId="38" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="26" borderId="35" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="62" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="58" fillId="31" borderId="10" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="50" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="50" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="26" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="58" fillId="31" borderId="30" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="58" fillId="31" borderId="34" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="58" fillId="31" borderId="35" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="30" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="30" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="65" fillId="30" borderId="10" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="30" borderId="33" xfId="50" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="65" fillId="30" borderId="29" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="30" borderId="30" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="30" borderId="33" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="30" borderId="30" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="29" borderId="35" xfId="50" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="26" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="58" fillId="31" borderId="38" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="50" applyFont="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="10" xfId="50" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="33" xfId="50" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="10" xfId="50" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="58" fillId="31" borderId="10" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3132,471 +3263,6 @@
   </cellStyles>
   <dxfs count="120">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF0E84A0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="22"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor indexed="43"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3651,6 +3317,471 @@
           <bgColor indexed="57"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF0E84A0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -5593,8 +5724,8 @@
     </indexedColors>
     <mruColors>
       <color rgb="FF00FFFF"/>
+      <color rgb="FF0E84A0"/>
       <color rgb="FFC0C0C0"/>
-      <color rgb="FF0E84A0"/>
       <color rgb="FFCCFFFF"/>
       <color rgb="FFFFFF99"/>
     </mruColors>
@@ -6906,6 +7037,1007 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Performance (Angular)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Moods Median Test'!$Q$2:$Q$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Moods Median Test'!$R$2:$R$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6631-C743-AF12-17E78414CF2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="860688383"/>
+        <c:axId val="860608895"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="860688383"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bins (Limits)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="860608895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="860608895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="860688383"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Performance (React)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Moods Median Test'!$T$2:$T$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Moods Median Test'!$U$2:$U$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1453-D547-9712-FD974E787E7E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="508338639"/>
+        <c:axId val="508218815"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="508338639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Bin (Limits)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508218815"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="508218815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frequency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="508338639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr/>
@@ -7658,6 +8790,1092 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -7702,6 +9920,83 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>169334</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>224366</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>270934</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E297E7EE-3A4F-0C75-CD11-AF20DBECA102}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>563032</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>215899</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1AED540-5757-ACE1-CDE9-9CC160E628CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
@@ -7994,20 +10289,20 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table3" displayName="Table3" ref="A1:F50" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table3" displayName="Table3" ref="A1:F50" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Xi" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Xi" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Median"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Diff= (Yi-Xi)" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Diff= (Yi-Xi)" dataDxfId="25">
       <calculatedColumnFormula>IF(A2="",NA(),B$2-A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Abs(Diff)" dataDxfId="20">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Abs(Diff)" dataDxfId="24">
       <calculatedColumnFormula>IF(A2="","",ABS(C2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Rank" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Rank" dataDxfId="23">
       <calculatedColumnFormula>IF(A2="","",IF(COUNTIF($D:$D,"="&amp;D2)&gt;1,(((RANK(D2,$D:$D,1)+COUNTIF($D:$D,"="&amp;D2))*(RANK(D2,$D:$D,1)+COUNTIF($D:$D,"="&amp;D2)-1))/2-(RANK(D2,$D:$D,1)*(RANK(D2,$D:$D,1)-1))/2)/COUNTIF($D:$D,"="&amp;D2),RANK(D2,$D:$D,1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Signed Rank" dataDxfId="18">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Signed Rank" dataDxfId="22">
       <calculatedColumnFormula>IF(A2="",NA(),SIGN(C2)*E2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8016,20 +10311,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="20" tableBorderDxfId="19" totalsRowBorderDxfId="18">
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Xi" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Yi" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Diff= (Yi-Xi)" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Xi" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Yi" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Diff= (Yi-Xi)" dataDxfId="15">
       <calculatedColumnFormula>IF(A2="",NA(),B2-A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Abs(Diff)" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Abs(Diff)" dataDxfId="14">
       <calculatedColumnFormula>IF(A2="","",ABS(C2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Rank" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Rank" dataDxfId="13">
       <calculatedColumnFormula>IF(A2="","",IF(COUNTIF($D:$D,"="&amp;D2)&gt;1,(((RANK(D2,$D:$D,1)+COUNTIF($D:$D,"="&amp;D2))*(RANK(D2,$D:$D,1)+COUNTIF($D:$D,"="&amp;D2)-1))/2-(RANK(D2,$D:$D,1)*(RANK(D2,$D:$D,1)-1))/2)/COUNTIF($D:$D,"="&amp;D2),RANK(D2,$D:$D,1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Signed Rank" dataDxfId="8">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Signed Rank" dataDxfId="12">
       <calculatedColumnFormula>IF(A2="",NA(),SIGN(C2)*E2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8038,14 +10333,14 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table2" displayName="Table2" ref="A1:D50" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table2" displayName="Table2" ref="A1:D50" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Sample 1" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Sample 2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Rank 1" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Sample 1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Sample 2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Rank 1" dataDxfId="5">
       <calculatedColumnFormula>RANK(A2,($A:$A,$B:$B),1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Rank 2" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Rank 2" dataDxfId="4">
       <calculatedColumnFormula>RANK(B2,($A:$A,$B:$B),1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8449,11 +10744,11 @@
     <row r="1" spans="1:7" ht="57" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="279"/>
       <c r="B1" s="249"/>
-      <c r="C1" s="325" t="s">
+      <c r="C1" s="313" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="326"/>
-      <c r="E1" s="327"/>
+      <c r="D1" s="314"/>
+      <c r="E1" s="315"/>
       <c r="F1" s="278" t="s">
         <v>212</v>
       </c>
@@ -8479,15 +10774,15 @@
       <c r="G2" s="206"/>
     </row>
     <row r="3" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="328" t="s">
+      <c r="A3" s="316" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="329"/>
+      <c r="B3" s="317"/>
       <c r="C3" s="272"/>
       <c r="D3" s="297" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="323" t="s">
+      <c r="E3" s="311" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="273" t="s">
@@ -8496,24 +10791,24 @@
       <c r="G3" s="207"/>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="330"/>
-      <c r="B4" s="331"/>
+      <c r="A4" s="318"/>
+      <c r="B4" s="319"/>
       <c r="C4" s="238"/>
       <c r="D4" s="254" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="324"/>
+      <c r="E4" s="312"/>
       <c r="F4" s="273" t="s">
         <v>182</v>
       </c>
       <c r="G4" s="207"/>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="332"/>
-      <c r="B5" s="333"/>
+      <c r="A5" s="320"/>
+      <c r="B5" s="321"/>
       <c r="C5" s="238"/>
       <c r="D5" s="254" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E5" s="294"/>
       <c r="F5" s="273"/>
@@ -8805,7 +11100,7 @@
       <c r="A27" s="244"/>
       <c r="B27" s="238"/>
       <c r="C27" s="256" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D27" s="238" t="s">
         <v>28</v>
@@ -8813,7 +11108,7 @@
       <c r="E27" s="238"/>
       <c r="F27" s="240"/>
       <c r="G27" s="255" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
@@ -9314,10 +11609,10 @@
         <f>IF(Tukey!$B$5="","",Tukey!$B$5)</f>
         <v>17.100000000000001</v>
       </c>
-      <c r="D12" s="334" t="s">
+      <c r="D12" s="322" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="335"/>
+      <c r="E12" s="323"/>
       <c r="L12">
         <v>2</v>
       </c>
@@ -10235,20 +12530,20 @@
     <mergeCell ref="D12:E12"/>
   </mergeCells>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E10">
-    <cfRule type="expression" dxfId="27" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$D3=$E$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>$D11&lt;=$E$15</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20040,7 +22335,7 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F15" s="306">
+      <c r="F15" s="305">
         <f>ABS(F7-F10)/F11</f>
         <v>0.3077287274483318</v>
       </c>
@@ -20065,11 +22360,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F16" s="301">
+      <c r="F16" s="300">
         <f>2*(1-NORMSDIST(ABS(F15)))</f>
         <v>0.75828875843321075</v>
       </c>
-      <c r="G16" s="302" t="s">
+      <c r="G16" s="301" t="s">
         <v>49</v>
       </c>
       <c r="K16" s="1">
@@ -20090,14 +22385,14 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="F17" s="303" t="str">
+      <c r="F17" s="302" t="str">
         <f>IF($F$15&lt;NORMSINV(1-F14/2),"Cannot Reject Null Hypothesis at alpha="&amp;F14,"Reject Null Hypothesis at alpha="&amp;F14)</f>
         <v>Cannot Reject Null Hypothesis at alpha=0.05</v>
       </c>
-      <c r="G17" s="304"/>
-      <c r="H17" s="304"/>
-      <c r="I17" s="304"/>
-      <c r="J17" s="305"/>
+      <c r="G17" s="303"/>
+      <c r="H17" s="303"/>
+      <c r="I17" s="303"/>
+      <c r="J17" s="304"/>
       <c r="K17" s="1">
         <v>72</v>
       </c>
@@ -20586,10 +22881,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF99"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20601,386 +22896,818 @@
     <col min="5" max="5" width="9.83203125" style="299" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" style="299" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" style="299" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="299" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="299" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="299" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1640625" style="299"/>
+    <col min="8" max="8" width="14.1640625" style="299" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="299" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" style="299" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" style="299"/>
+    <col min="12" max="12" width="13" style="299" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="299" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14" style="299" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" style="299" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="299"/>
+    <col min="17" max="17" width="10.83203125" style="299" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" style="299" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1640625" style="299"/>
+    <col min="20" max="20" width="10" style="299" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" style="299" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1640625" style="299"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="A1" s="313" t="s">
+    <row r="1" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A1" s="309" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="309" t="s">
         <v>250</v>
       </c>
-      <c r="B1" s="313" t="s">
+      <c r="C1" s="306"/>
+      <c r="D1" s="309" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="330">
+        <v>8.57</v>
+      </c>
+      <c r="F1" s="331"/>
+      <c r="G1" s="332"/>
+      <c r="H1" s="339"/>
+      <c r="I1" s="340" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="307"/>
-      <c r="D1" s="314" t="s">
-        <v>246</v>
-      </c>
-      <c r="E1" s="310">
-        <f>SUM(H13:I14)</f>
-        <v>8.5714285714285712</v>
-      </c>
-      <c r="F1" s="307"/>
-      <c r="G1" s="307"/>
-      <c r="H1" s="313" t="str">
+      <c r="J1" s="340"/>
+      <c r="K1" s="338"/>
+      <c r="L1" s="332"/>
+      <c r="M1" s="333" t="s">
+        <v>242</v>
+      </c>
+      <c r="N1" s="309" t="s">
+        <v>249</v>
+      </c>
+      <c r="O1" s="309" t="s">
+        <v>250</v>
+      </c>
+      <c r="P1" s="332"/>
+      <c r="Q1" s="350" t="s">
+        <v>257</v>
+      </c>
+      <c r="R1" s="350" t="s">
+        <v>258</v>
+      </c>
+      <c r="S1" s="306"/>
+      <c r="T1" s="350" t="s">
+        <v>256</v>
+      </c>
+      <c r="U1" s="350" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="310">
+        <v>99</v>
+      </c>
+      <c r="B2" s="310">
+        <v>97</v>
+      </c>
+      <c r="C2" s="306"/>
+      <c r="D2" s="309" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="330">
+        <v>3.84</v>
+      </c>
+      <c r="F2" s="331"/>
+      <c r="G2" s="332"/>
+      <c r="H2" s="332"/>
+      <c r="I2" s="332"/>
+      <c r="J2" s="332"/>
+      <c r="K2" s="332"/>
+      <c r="L2" s="332"/>
+      <c r="M2" s="324" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" s="348">
+        <f>IF(A2="","",MEDIAN(A:A))</f>
+        <v>99</v>
+      </c>
+      <c r="O2" s="348">
+        <f>IF(B2="","",MEDIAN(B:B))</f>
+        <v>97</v>
+      </c>
+      <c r="P2" s="332"/>
+      <c r="Q2" s="351">
+        <v>80</v>
+      </c>
+      <c r="R2" s="350" cm="1">
+        <f t="array" ref="R2:R23">FREQUENCY(A2:A11,Q2:Q22)</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="306"/>
+      <c r="T2" s="351">
+        <v>80</v>
+      </c>
+      <c r="U2" s="350" cm="1">
+        <f t="array" ref="U2:U23">FREQUENCY(B2:B11,T2:T22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="310">
+        <v>86</v>
+      </c>
+      <c r="B3" s="310">
+        <v>97</v>
+      </c>
+      <c r="C3" s="306"/>
+      <c r="D3" s="334" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="353" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
+      <c r="H3" s="309" t="str">
         <f>A1</f>
         <v>Angular</v>
       </c>
-      <c r="I1" s="313" t="str">
+      <c r="I3" s="309" t="str">
         <f>B1</f>
         <v>React</v>
       </c>
-      <c r="J1" s="313" t="s">
+      <c r="J3" s="309" t="s">
         <v>245</v>
       </c>
-      <c r="L1" s="300" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A2" s="315">
-        <v>99</v>
-      </c>
-      <c r="B2" s="315">
+      <c r="K3" s="332"/>
+      <c r="L3" s="332"/>
+      <c r="M3" s="309" t="s">
+        <v>244</v>
+      </c>
+      <c r="N3" s="330">
+        <f>MEDIAN(A:B)</f>
         <v>97</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="316" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="317">
-        <f ca="1">_xlfn.CHISQ.TEST(OFFSET(H2,0,0,2,COUNT(H8:I8)),OFFSET(H8,0,0,2,COUNT(H8:I8)))</f>
-        <v>3.4147911781178169E-3</v>
-      </c>
-      <c r="F2" s="307"/>
-      <c r="G2" s="313" t="s">
-        <v>248</v>
-      </c>
-      <c r="H2" s="309">
+      <c r="O3" s="331"/>
+      <c r="P3" s="332"/>
+      <c r="Q3" s="351">
+        <f>Q2+1</f>
+        <v>81</v>
+      </c>
+      <c r="R3" s="350">
+        <v>0</v>
+      </c>
+      <c r="S3" s="306"/>
+      <c r="T3" s="351">
+        <f>T2+1</f>
+        <v>81</v>
+      </c>
+      <c r="U3" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="310">
+        <v>86</v>
+      </c>
+      <c r="B4" s="310">
+        <v>97</v>
+      </c>
+      <c r="C4" s="306"/>
+      <c r="D4" s="347" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="346">
+        <v>0.05</v>
+      </c>
+      <c r="F4" s="331"/>
+      <c r="G4" s="309" t="s">
+        <v>247</v>
+      </c>
+      <c r="H4" s="330">
         <f>IF(A2="","",COUNTIF(A:A,"&gt;"&amp;MEDIAN($A:$B)))</f>
         <v>6</v>
       </c>
-      <c r="I2" s="309">
+      <c r="I4" s="330">
         <f>IF(B2="","",COUNTIF(B:B,"&gt;"&amp;MEDIAN($A:$B)))</f>
         <v>0</v>
       </c>
-      <c r="J2" s="309">
-        <f>SUM(H2:I2)</f>
+      <c r="J4" s="330">
+        <f>SUM(H4:I4)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A3" s="315">
+      <c r="K4" s="332"/>
+      <c r="L4" s="332"/>
+      <c r="M4" s="332"/>
+      <c r="N4" s="332"/>
+      <c r="O4" s="332"/>
+      <c r="P4" s="332"/>
+      <c r="Q4" s="351">
+        <f t="shared" ref="Q4:Q22" si="0">Q3+1</f>
+        <v>82</v>
+      </c>
+      <c r="R4" s="350">
+        <v>0</v>
+      </c>
+      <c r="S4" s="306"/>
+      <c r="T4" s="351">
+        <f t="shared" ref="T4:T22" si="1">T3+1</f>
+        <v>82</v>
+      </c>
+      <c r="U4" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="310">
+        <v>99</v>
+      </c>
+      <c r="B5" s="310">
+        <v>84</v>
+      </c>
+      <c r="C5" s="306"/>
+      <c r="D5" s="344" t="str">
+        <f>IF(E3&lt;E4,"Variables are Related","Variables are Independent")</f>
+        <v>Variables are Independent</v>
+      </c>
+      <c r="E5" s="345"/>
+      <c r="F5" s="331"/>
+      <c r="G5" s="309" t="s">
+        <v>248</v>
+      </c>
+      <c r="H5" s="330">
+        <f>IF(H4="","",COUNT(A:A)-H4)</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="330">
+        <f>IF(I4="","",COUNT(B:B)-I4)</f>
+        <v>10</v>
+      </c>
+      <c r="J5" s="330">
+        <f>SUM(H5:I5)</f>
+        <v>14</v>
+      </c>
+      <c r="K5" s="332"/>
+      <c r="L5" s="332"/>
+      <c r="M5" s="332"/>
+      <c r="N5" s="332"/>
+      <c r="O5" s="332"/>
+      <c r="P5" s="332"/>
+      <c r="Q5" s="351">
+        <f t="shared" si="0"/>
+        <v>83</v>
+      </c>
+      <c r="R5" s="350">
+        <v>0</v>
+      </c>
+      <c r="S5" s="306"/>
+      <c r="T5" s="351">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="U5" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="310">
+        <v>84</v>
+      </c>
+      <c r="B6" s="310">
+        <v>97</v>
+      </c>
+      <c r="C6" s="306"/>
+      <c r="D6" s="331"/>
+      <c r="E6" s="331"/>
+      <c r="F6" s="331"/>
+      <c r="G6" s="309" t="s">
+        <v>245</v>
+      </c>
+      <c r="H6" s="330">
+        <f>SUM(H4:H5)</f>
+        <v>10</v>
+      </c>
+      <c r="I6" s="330">
+        <f>SUM(I4:I5)</f>
+        <v>10</v>
+      </c>
+      <c r="J6" s="330">
+        <f>SUM(H6:I6)</f>
+        <v>20</v>
+      </c>
+      <c r="K6" s="332"/>
+      <c r="L6" s="332"/>
+      <c r="M6" s="332"/>
+      <c r="N6" s="332"/>
+      <c r="O6" s="332"/>
+      <c r="P6" s="332"/>
+      <c r="Q6" s="351">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="R6" s="350">
+        <v>1</v>
+      </c>
+      <c r="S6" s="306"/>
+      <c r="T6" s="351">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="U6" s="350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="310">
+        <v>99</v>
+      </c>
+      <c r="B7" s="310">
+        <v>97</v>
+      </c>
+      <c r="C7" s="306"/>
+      <c r="D7" s="331"/>
+      <c r="E7" s="331"/>
+      <c r="F7" s="331"/>
+      <c r="L7" s="332"/>
+      <c r="M7" s="332"/>
+      <c r="N7" s="332"/>
+      <c r="O7" s="332"/>
+      <c r="P7" s="332"/>
+      <c r="Q7" s="351">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="R7" s="350">
+        <v>0</v>
+      </c>
+      <c r="S7" s="306"/>
+      <c r="T7" s="351">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="U7" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="310">
+        <v>99</v>
+      </c>
+      <c r="B8" s="310">
+        <v>97</v>
+      </c>
+      <c r="C8" s="306"/>
+      <c r="D8" s="331"/>
+      <c r="E8" s="331"/>
+      <c r="F8" s="331"/>
+      <c r="G8" s="331"/>
+      <c r="H8" s="341"/>
+      <c r="I8" s="342" t="s">
+        <v>252</v>
+      </c>
+      <c r="J8" s="343"/>
+      <c r="K8" s="338"/>
+      <c r="L8" s="332"/>
+      <c r="M8" s="332"/>
+      <c r="N8" s="332"/>
+      <c r="O8" s="332"/>
+      <c r="P8" s="332"/>
+      <c r="Q8" s="351">
+        <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="B3" s="315">
+      <c r="R8" s="350">
+        <v>3</v>
+      </c>
+      <c r="S8" s="306"/>
+      <c r="T8" s="351">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="U8" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="310">
+        <v>99</v>
+      </c>
+      <c r="B9" s="310">
         <v>97</v>
       </c>
-      <c r="C3" s="307"/>
-      <c r="D3" s="318" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" s="308">
-        <v>0.05</v>
-      </c>
-      <c r="F3" s="307"/>
-      <c r="G3" s="313" t="s">
-        <v>249</v>
-      </c>
-      <c r="H3" s="309">
-        <f>IF(H2="","",COUNT(A:A)-H2)</f>
-        <v>4</v>
-      </c>
-      <c r="I3" s="309">
-        <f>IF(I2="","",COUNT(B:B)-I2)</f>
+      <c r="C9" s="306"/>
+      <c r="D9" s="331"/>
+      <c r="E9" s="331"/>
+      <c r="F9" s="331"/>
+      <c r="G9" s="331"/>
+      <c r="H9" s="326"/>
+      <c r="I9" s="326"/>
+      <c r="J9" s="326"/>
+      <c r="K9" s="332"/>
+      <c r="L9" s="332"/>
+      <c r="M9" s="332"/>
+      <c r="N9" s="332"/>
+      <c r="O9" s="332"/>
+      <c r="P9" s="332"/>
+      <c r="Q9" s="351">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="R9" s="350">
+        <v>0</v>
+      </c>
+      <c r="S9" s="306"/>
+      <c r="T9" s="351">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="U9" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="310">
+        <v>99</v>
+      </c>
+      <c r="B10" s="310">
+        <v>97</v>
+      </c>
+      <c r="C10" s="306"/>
+      <c r="D10" s="331"/>
+      <c r="E10" s="328"/>
+      <c r="F10" s="328"/>
+      <c r="G10" s="331"/>
+      <c r="H10" s="309" t="str">
+        <f>H3</f>
+        <v>Angular</v>
+      </c>
+      <c r="I10" s="309" t="str">
+        <f>I3</f>
+        <v>React</v>
+      </c>
+      <c r="J10" s="309" t="s">
+        <v>245</v>
+      </c>
+      <c r="K10" s="332"/>
+      <c r="L10" s="332"/>
+      <c r="M10" s="332"/>
+      <c r="N10" s="332"/>
+      <c r="O10" s="332"/>
+      <c r="P10" s="332"/>
+      <c r="Q10" s="351">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="R10" s="350">
+        <v>0</v>
+      </c>
+      <c r="S10" s="306"/>
+      <c r="T10" s="351">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="U10" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="310">
+        <v>86</v>
+      </c>
+      <c r="B11" s="310">
+        <v>97</v>
+      </c>
+      <c r="C11" s="306"/>
+      <c r="D11" s="331"/>
+      <c r="E11" s="328"/>
+      <c r="F11" s="328"/>
+      <c r="G11" s="309" t="str">
+        <f>G4</f>
+        <v>&gt; Median</v>
+      </c>
+      <c r="H11" s="335">
+        <f>(H$6*$J$4)/$J$6</f>
+        <v>3</v>
+      </c>
+      <c r="I11" s="330">
+        <f>(I$6*$J$4)/$J$6</f>
+        <v>3</v>
+      </c>
+      <c r="J11" s="330">
+        <f>SUM(H11:I11)</f>
+        <v>6</v>
+      </c>
+      <c r="K11" s="332"/>
+      <c r="L11" s="332"/>
+      <c r="M11" s="332"/>
+      <c r="N11" s="332"/>
+      <c r="O11" s="332"/>
+      <c r="P11" s="332"/>
+      <c r="Q11" s="351">
+        <f t="shared" si="0"/>
+        <v>89</v>
+      </c>
+      <c r="R11" s="350">
+        <v>0</v>
+      </c>
+      <c r="S11" s="306"/>
+      <c r="T11" s="351">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="U11" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A12" s="308"/>
+      <c r="B12" s="308"/>
+      <c r="C12" s="306"/>
+      <c r="D12" s="331"/>
+      <c r="E12" s="328"/>
+      <c r="F12" s="328"/>
+      <c r="G12" s="325" t="str">
+        <f>G5</f>
+        <v>&lt;= Median</v>
+      </c>
+      <c r="H12" s="336">
+        <f>(H$6*$J$5)/$J$6</f>
+        <v>7</v>
+      </c>
+      <c r="I12" s="337">
+        <f>(I$6*$J$5)/$J$6</f>
+        <v>7</v>
+      </c>
+      <c r="J12" s="337">
+        <f>SUM(H12:I12)</f>
+        <v>14</v>
+      </c>
+      <c r="K12" s="332"/>
+      <c r="L12" s="332"/>
+      <c r="M12" s="332"/>
+      <c r="N12" s="332"/>
+      <c r="O12" s="332"/>
+      <c r="P12" s="332"/>
+      <c r="Q12" s="351">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="R12" s="350">
+        <v>0</v>
+      </c>
+      <c r="S12" s="306"/>
+      <c r="T12" s="351">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="U12" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A13" s="308"/>
+      <c r="B13" s="308"/>
+      <c r="C13" s="306"/>
+      <c r="D13" s="331"/>
+      <c r="E13" s="328"/>
+      <c r="F13" s="328"/>
+      <c r="G13" s="309" t="s">
+        <v>245</v>
+      </c>
+      <c r="H13" s="330">
         <v>10</v>
       </c>
-      <c r="J3" s="309">
-        <f>SUM(H3:I3)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A4" s="315">
-        <v>86</v>
-      </c>
-      <c r="B4" s="315">
+      <c r="I13" s="330">
+        <v>10</v>
+      </c>
+      <c r="J13" s="330">
+        <v>20</v>
+      </c>
+      <c r="K13" s="332"/>
+      <c r="L13" s="332"/>
+      <c r="M13" s="332"/>
+      <c r="N13" s="332"/>
+      <c r="O13" s="332"/>
+      <c r="P13" s="332"/>
+      <c r="Q13" s="351">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="R13" s="350">
+        <v>0</v>
+      </c>
+      <c r="S13" s="306"/>
+      <c r="T13" s="351">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+      <c r="U13" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A14" s="308"/>
+      <c r="B14" s="308"/>
+      <c r="C14" s="306"/>
+      <c r="D14" s="306"/>
+      <c r="E14" s="327"/>
+      <c r="F14" s="327"/>
+      <c r="G14" s="326" t="str">
+        <f>G5</f>
+        <v>&lt;= Median</v>
+      </c>
+      <c r="H14" s="329">
+        <f>IF(H12="","",(H5-H12)^2/H12)</f>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="I14" s="329">
+        <f>IF(I12="","",(I5-I12)^2/I12)</f>
+        <v>1.2857142857142858</v>
+      </c>
+      <c r="J14" s="327"/>
+      <c r="Q14" s="351">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="R14" s="350">
+        <v>0</v>
+      </c>
+      <c r="S14" s="306"/>
+      <c r="T14" s="351">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+      <c r="U14" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A15" s="308"/>
+      <c r="B15" s="308"/>
+      <c r="C15" s="306"/>
+      <c r="D15" s="306"/>
+      <c r="E15" s="327"/>
+      <c r="F15" s="327"/>
+      <c r="G15" s="327"/>
+      <c r="H15" s="327"/>
+      <c r="I15" s="327"/>
+      <c r="J15" s="327"/>
+      <c r="Q15" s="351">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="R15" s="350">
+        <v>0</v>
+      </c>
+      <c r="S15" s="306"/>
+      <c r="T15" s="351">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+      <c r="U15" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A16" s="308"/>
+      <c r="B16" s="308"/>
+      <c r="C16" s="306"/>
+      <c r="D16" s="306"/>
+      <c r="E16" s="306"/>
+      <c r="F16" s="306"/>
+      <c r="J16" s="306"/>
+      <c r="Q16" s="351">
+        <f>Q15+1</f>
+        <v>94</v>
+      </c>
+      <c r="R16" s="350">
+        <v>0</v>
+      </c>
+      <c r="S16" s="349"/>
+      <c r="T16" s="351">
+        <f>T15+1</f>
+        <v>94</v>
+      </c>
+      <c r="U16" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="A17" s="308"/>
+      <c r="B17" s="308"/>
+      <c r="C17" s="306"/>
+      <c r="D17" s="306"/>
+      <c r="E17" s="306"/>
+      <c r="F17" s="306"/>
+      <c r="J17" s="307"/>
+      <c r="Q17" s="351">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+      <c r="R17" s="350">
+        <v>0</v>
+      </c>
+      <c r="S17" s="349"/>
+      <c r="T17" s="351">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="U17" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="Q18" s="351">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+      <c r="R18" s="350">
+        <v>0</v>
+      </c>
+      <c r="S18" s="349"/>
+      <c r="T18" s="351">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="U18" s="350">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="25" x14ac:dyDescent="0.25">
+      <c r="Q19" s="351">
+        <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="C4" s="307"/>
-      <c r="D4" s="319" t="str">
-        <f ca="1">IF(E2&lt;E3,"Variables are Related","Variables are Independent")</f>
-        <v>Variables are Related</v>
-      </c>
-      <c r="E4" s="319"/>
-      <c r="F4" s="307"/>
-      <c r="G4" s="313" t="s">
-        <v>245</v>
-      </c>
-      <c r="H4" s="309">
-        <f>SUM(H2:H3)</f>
-        <v>10</v>
-      </c>
-      <c r="I4" s="309">
-        <f>SUM(I2:I3)</f>
-        <v>10</v>
-      </c>
-      <c r="J4" s="309">
-        <f>SUM(H4:I4)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A5" s="315">
+      <c r="R19" s="350">
+        <v>0</v>
+      </c>
+      <c r="S19" s="349"/>
+      <c r="T19" s="351">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+      <c r="U19" s="350">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="Q20" s="351">
+        <f>Q19+1</f>
+        <v>98</v>
+      </c>
+      <c r="R20" s="350">
+        <v>0</v>
+      </c>
+      <c r="T20" s="351">
+        <f>T19+1</f>
+        <v>98</v>
+      </c>
+      <c r="U20" s="352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="Q21" s="351">
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="B5" s="315">
-        <v>84</v>
-      </c>
-      <c r="C5" s="307"/>
-      <c r="D5" s="307"/>
-      <c r="E5" s="307"/>
-      <c r="F5" s="307"/>
-      <c r="G5" s="307"/>
-      <c r="H5" s="307"/>
-      <c r="I5" s="307"/>
-      <c r="J5" s="307"/>
-    </row>
-    <row r="6" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A6" s="315">
-        <v>84</v>
-      </c>
-      <c r="B6" s="315">
-        <v>97</v>
-      </c>
-      <c r="C6" s="307"/>
-      <c r="D6" s="307"/>
-      <c r="E6" s="307"/>
-      <c r="F6" s="307"/>
-      <c r="G6" s="307"/>
-      <c r="H6" s="320"/>
-      <c r="I6" s="320"/>
-      <c r="J6" s="307"/>
-    </row>
-    <row r="7" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A7" s="315">
+      <c r="R21" s="350">
+        <v>6</v>
+      </c>
+      <c r="T21" s="351">
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B7" s="315">
-        <v>97</v>
-      </c>
-      <c r="C7" s="307"/>
-      <c r="D7" s="307"/>
-      <c r="E7" s="307"/>
-      <c r="F7" s="307"/>
-      <c r="G7" s="307"/>
-      <c r="H7" s="321" t="str">
-        <f>H1</f>
-        <v>Angular</v>
-      </c>
-      <c r="I7" s="321" t="str">
-        <f>I1</f>
-        <v>React</v>
-      </c>
-      <c r="J7" s="307"/>
-    </row>
-    <row r="8" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A8" s="315">
-        <v>99</v>
-      </c>
-      <c r="B8" s="315">
-        <v>97</v>
-      </c>
-      <c r="C8" s="307"/>
-      <c r="D8" s="307"/>
-      <c r="E8" s="307"/>
-      <c r="F8" s="307"/>
-      <c r="G8" s="313" t="str">
-        <f>G2</f>
-        <v>&gt; Median</v>
-      </c>
-      <c r="H8" s="322">
-        <f>(H$4*$J$2)/$J$4</f>
-        <v>3</v>
-      </c>
-      <c r="I8" s="310">
-        <f>(I$4*$J$2)/$J$4</f>
-        <v>3</v>
-      </c>
-      <c r="J8" s="307"/>
-    </row>
-    <row r="9" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A9" s="315">
-        <v>99</v>
-      </c>
-      <c r="B9" s="315">
-        <v>97</v>
-      </c>
-      <c r="C9" s="307"/>
-      <c r="D9" s="307"/>
-      <c r="E9" s="307"/>
-      <c r="F9" s="307"/>
-      <c r="G9" s="313" t="str">
-        <f>G3</f>
-        <v>&lt;= Median</v>
-      </c>
-      <c r="H9" s="322">
-        <f>(H$4*$J$3)/$J$4</f>
-        <v>7</v>
-      </c>
-      <c r="I9" s="310">
-        <f>(I$4*$J$3)/$J$4</f>
-        <v>7</v>
-      </c>
-      <c r="J9" s="307"/>
-    </row>
-    <row r="10" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A10" s="315">
-        <v>99</v>
-      </c>
-      <c r="B10" s="315">
-        <v>97</v>
-      </c>
-      <c r="C10" s="307"/>
-      <c r="D10" s="307"/>
-      <c r="E10" s="307"/>
-      <c r="F10" s="307"/>
-      <c r="G10" s="307"/>
-      <c r="H10" s="307"/>
-      <c r="I10" s="307"/>
-      <c r="J10" s="307"/>
-    </row>
-    <row r="11" spans="1:12" ht="26" x14ac:dyDescent="0.3">
-      <c r="A11" s="315">
-        <v>86</v>
-      </c>
-      <c r="B11" s="315">
-        <v>97</v>
-      </c>
-      <c r="C11" s="307"/>
-      <c r="D11" s="307"/>
-      <c r="E11" s="307"/>
-      <c r="F11" s="307"/>
-      <c r="G11" s="307"/>
-      <c r="H11" s="320"/>
-      <c r="I11" s="320"/>
-      <c r="J11" s="307"/>
-    </row>
-    <row r="12" spans="1:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="A12" s="312"/>
-      <c r="B12" s="312"/>
-      <c r="C12" s="307"/>
-      <c r="D12" s="307"/>
-      <c r="E12" s="307"/>
-      <c r="F12" s="307"/>
-      <c r="G12" s="307"/>
-      <c r="H12" s="321" t="str">
-        <f>H1</f>
-        <v>Angular</v>
-      </c>
-      <c r="I12" s="321" t="str">
-        <f>I1</f>
-        <v>React</v>
-      </c>
-      <c r="J12" s="307"/>
-    </row>
-    <row r="13" spans="1:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="A13" s="312"/>
-      <c r="B13" s="312"/>
-      <c r="C13" s="307"/>
-      <c r="D13" s="307"/>
-      <c r="E13" s="307"/>
-      <c r="F13" s="307"/>
-      <c r="G13" s="313" t="str">
-        <f>G2</f>
-        <v>&gt; Median</v>
-      </c>
-      <c r="H13" s="310">
-        <f t="shared" ref="H13:I14" si="0">IF(H8="","",(H2-H8)^2/H8)</f>
-        <v>3</v>
-      </c>
-      <c r="I13" s="310">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J13" s="307"/>
-    </row>
-    <row r="14" spans="1:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="A14" s="312"/>
-      <c r="B14" s="312"/>
-      <c r="C14" s="307"/>
-      <c r="D14" s="307"/>
-      <c r="E14" s="307"/>
-      <c r="F14" s="307"/>
-      <c r="G14" s="313" t="str">
-        <f>G3</f>
-        <v>&lt;= Median</v>
-      </c>
-      <c r="H14" s="310">
-        <f t="shared" si="0"/>
-        <v>1.2857142857142858</v>
-      </c>
-      <c r="I14" s="310">
-        <f t="shared" si="0"/>
-        <v>1.2857142857142858</v>
-      </c>
-      <c r="J14" s="307"/>
-    </row>
-    <row r="15" spans="1:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="A15" s="312"/>
-      <c r="B15" s="312"/>
-      <c r="C15" s="307"/>
-      <c r="D15" s="307"/>
-      <c r="E15" s="307"/>
-      <c r="F15" s="307"/>
-      <c r="G15" s="307"/>
-      <c r="H15" s="307"/>
-      <c r="I15" s="307"/>
-      <c r="J15" s="307"/>
-    </row>
-    <row r="16" spans="1:12" ht="25" x14ac:dyDescent="0.25">
-      <c r="A16" s="312"/>
-      <c r="B16" s="312"/>
-      <c r="C16" s="307"/>
-      <c r="D16" s="307"/>
-      <c r="E16" s="307"/>
-      <c r="F16" s="307"/>
-      <c r="G16" s="313" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="309">
-        <f>IF(A2="","",MEDIAN(A:A))</f>
-        <v>99</v>
-      </c>
-      <c r="I16" s="309">
-        <f>IF(B2="","",MEDIAN(B:B))</f>
-        <v>97</v>
-      </c>
-      <c r="J16" s="307"/>
-    </row>
-    <row r="17" spans="1:10" ht="25" x14ac:dyDescent="0.25">
-      <c r="A17" s="312"/>
-      <c r="B17" s="312"/>
-      <c r="C17" s="307"/>
-      <c r="D17" s="307"/>
-      <c r="E17" s="307"/>
-      <c r="F17" s="307"/>
-      <c r="G17" s="313" t="s">
-        <v>244</v>
-      </c>
-      <c r="H17" s="309">
-        <f>MEDIAN(A:B)</f>
-        <v>97</v>
-      </c>
-      <c r="I17" s="307"/>
-      <c r="J17" s="311"/>
+      <c r="U21" s="352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="Q22" s="351">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="R22" s="350">
+        <v>0</v>
+      </c>
+      <c r="T22" s="351">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="U22" s="352">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="26" x14ac:dyDescent="0.3">
+      <c r="R23" s="350">
+        <v>0</v>
+      </c>
+      <c r="U23" s="352">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>